<commit_message>
Testing after reseting SciAv data, satellite code for Evan
</commit_message>
<xml_diff>
--- a/01_clean_reports/sciav_1_clean.xlsx
+++ b/01_clean_reports/sciav_1_clean.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/01_clean_reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5428782-9401-4B40-8B47-C23F991F8ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6384F0C-4D3E-0D4E-83D8-A31F845690E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41760" yWindow="520" windowWidth="27740" windowHeight="19540" xr2:uid="{AE40F39B-4EB9-E64E-9875-C52BE52916C0}"/>
+    <workbookView xWindow="38480" yWindow="1480" windowWidth="27740" windowHeight="19540" xr2:uid="{AE40F39B-4EB9-E64E-9875-C52BE52916C0}"/>
   </bookViews>
   <sheets>
     <sheet name="clean_report" sheetId="1" r:id="rId1"/>
     <sheet name="raw_report" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -214,7 +214,7 @@
     <t>SA-2</t>
   </si>
   <si>
-    <t>unknown</t>
+    <t>1-sigma</t>
   </si>
 </sst>
 </file>
@@ -222,8 +222,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="[h]:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="[h]:mm:ss;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -303,14 +303,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -318,7 +317,7 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -335,24 +334,24 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,7 +669,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:H19"/>
+      <selection activeCell="L2" sqref="L2:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,13 +739,13 @@
       <c r="D2" s="2">
         <v>44873</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="17">
         <v>0.90025462962962965</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="17">
         <v>0.92664351851851856</v>
       </c>
-      <c r="G2" s="4" t="b">
+      <c r="G2" t="b">
         <v>1</v>
       </c>
       <c r="H2" t="b">
@@ -787,13 +786,13 @@
       <c r="D3" s="2">
         <v>44873</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="17">
         <v>0.93903935185185183</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="17">
         <v>0.95562499999999995</v>
       </c>
-      <c r="G3" s="4" t="b">
+      <c r="G3" t="b">
         <v>1</v>
       </c>
       <c r="H3" t="b">
@@ -834,13 +833,13 @@
       <c r="D4" s="2">
         <v>44873</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="17">
         <v>0.96238425925925919</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="17">
         <v>0.9767824074074074</v>
       </c>
-      <c r="G4" s="4" t="b">
+      <c r="G4" t="b">
         <v>1</v>
       </c>
       <c r="H4" t="b">
@@ -881,14 +880,14 @@
       <c r="D5" s="2">
         <v>44873</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="17">
         <v>0.98979166666666663</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="17">
         <v>0.99689814814814814</v>
       </c>
-      <c r="G5" s="4" t="b">
-        <v>1</v>
+      <c r="G5" t="b">
+        <v>0</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
@@ -928,13 +927,13 @@
       <c r="D6" s="2">
         <v>44875</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="17">
         <v>0.75412037037037039</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="17">
         <v>0.76953703703703702</v>
       </c>
-      <c r="G6" s="4" t="b">
+      <c r="G6" t="b">
         <v>1</v>
       </c>
       <c r="H6" t="b">
@@ -975,13 +974,13 @@
       <c r="D7" s="2">
         <v>44875</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="17">
         <v>0.78233796296296287</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="17">
         <v>0.80181712962962959</v>
       </c>
-      <c r="G7" s="4" t="b">
+      <c r="G7" t="b">
         <v>1</v>
       </c>
       <c r="H7" t="b">
@@ -1022,13 +1021,13 @@
       <c r="D8" s="2">
         <v>44875</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="17">
         <v>0.8097685185185185</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="17">
         <v>0.82709490740740732</v>
       </c>
-      <c r="G8" s="4" t="b">
+      <c r="G8" t="b">
         <v>1</v>
       </c>
       <c r="H8" t="b">
@@ -1069,14 +1068,14 @@
       <c r="D9" s="2">
         <v>44875</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="17">
         <v>0.83679398148148154</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="17">
         <v>0.85003472222222232</v>
       </c>
-      <c r="G9" s="4" t="b">
-        <v>1</v>
+      <c r="G9" t="b">
+        <v>0</v>
       </c>
       <c r="H9" t="b">
         <v>1</v>
@@ -1116,13 +1115,13 @@
       <c r="D10" s="2">
         <v>44875</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="17">
         <v>0.86641203703703706</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="17">
         <v>0.88399305555555552</v>
       </c>
-      <c r="G10" s="4" t="b">
+      <c r="G10" t="b">
         <v>1</v>
       </c>
       <c r="H10" t="b">
@@ -1163,13 +1162,13 @@
       <c r="D11" s="2">
         <v>44875</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="17">
         <v>0.89293981481481488</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="17">
         <v>0.91015046296296298</v>
       </c>
-      <c r="G11" s="4" t="b">
+      <c r="G11" t="b">
         <v>1</v>
       </c>
       <c r="H11" t="b">
@@ -1210,13 +1209,13 @@
       <c r="D12" s="2">
         <v>44875</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="17">
         <v>0.91326388888888888</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="17">
         <v>0.9176157407407407</v>
       </c>
-      <c r="G12" s="4" t="b">
+      <c r="G12" t="b">
         <v>1</v>
       </c>
       <c r="H12" t="b">
@@ -1257,13 +1256,13 @@
       <c r="D13" s="2">
         <v>44876</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="17">
         <v>0.80180555555555555</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="17">
         <v>0.81092592592592594</v>
       </c>
-      <c r="G13" s="4" t="b">
+      <c r="G13" t="b">
         <v>1</v>
       </c>
       <c r="H13" t="b">
@@ -1304,13 +1303,13 @@
       <c r="D14" s="2">
         <v>44876</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="17">
         <v>0.82604166666666667</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="17">
         <v>0.83738425925925919</v>
       </c>
-      <c r="G14" s="4" t="b">
+      <c r="G14" t="b">
         <v>1</v>
       </c>
       <c r="H14" t="b">
@@ -1351,14 +1350,14 @@
       <c r="D15" s="2">
         <v>44876</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="17">
         <v>0.85099537037037043</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="17">
         <v>0.86252314814814823</v>
       </c>
-      <c r="G15" s="4" t="b">
-        <v>1</v>
+      <c r="G15" t="b">
+        <v>0</v>
       </c>
       <c r="H15" t="b">
         <v>1</v>
@@ -1398,13 +1397,13 @@
       <c r="D16" s="2">
         <v>44876</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="17">
         <v>0.87223379629629638</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="17">
         <v>0.88641203703703697</v>
       </c>
-      <c r="G16" s="4" t="b">
+      <c r="G16" t="b">
         <v>1</v>
       </c>
       <c r="H16" t="b">
@@ -1445,13 +1444,13 @@
       <c r="D17" s="2">
         <v>44876</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="17">
         <v>0.89629629629629637</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="17">
         <v>0.90858796296296296</v>
       </c>
-      <c r="G17" s="4" t="b">
+      <c r="G17" t="b">
         <v>0</v>
       </c>
       <c r="H17" t="b">
@@ -1492,13 +1491,13 @@
       <c r="D18" s="2">
         <v>44876</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="17">
         <v>0.94651620370370371</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="17">
         <v>0.96113425925925933</v>
       </c>
-      <c r="G18" s="4" t="b">
+      <c r="G18" t="b">
         <v>1</v>
       </c>
       <c r="H18" t="b">
@@ -1539,13 +1538,13 @@
       <c r="D19" s="2">
         <v>44876</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="17">
         <v>0.97072916666666664</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="17">
         <v>0.98579861111111111</v>
       </c>
-      <c r="G19" s="4" t="b">
+      <c r="G19" t="b">
         <v>1</v>
       </c>
       <c r="H19" t="b">
@@ -1589,30 +1588,30 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="19" t="s">
         <v>21</v>
       </c>
       <c r="L1" t="s">
@@ -1626,16 +1625,16 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="17"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -1644,35 +1643,35 @@
       <c r="B3" s="3">
         <v>44873</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>5</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>205</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>8.1999999999999993</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>77782</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <v>80062</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="21">
+      <c r="L3" s="16">
         <f>H3/86400</f>
         <v>0.90025462962962965</v>
       </c>
-      <c r="M3" s="21">
+      <c r="M3" s="16">
         <f>I3/86400</f>
         <v>0.92664351851851856</v>
       </c>
@@ -1681,41 +1680,41 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>7</v>
       </c>
       <c r="B4" s="3">
         <v>44873</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>140</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>102</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>207</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>7.2</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>81133</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>82566</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="21">
+      <c r="L4" s="16">
         <f t="shared" ref="L4:L22" si="0">H4/86400</f>
         <v>0.93903935185185183</v>
       </c>
-      <c r="M4" s="21">
+      <c r="M4" s="16">
         <f t="shared" ref="M4:M22" si="1">I4/86400</f>
         <v>0.95562499999999995</v>
       </c>
@@ -1724,41 +1723,41 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>8</v>
       </c>
       <c r="B5" s="3">
         <v>44873</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>8</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>4</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>209</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>7.6</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>83150</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>84394</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="21">
+      <c r="L5" s="16">
         <f t="shared" si="0"/>
         <v>0.9623842592592593</v>
       </c>
-      <c r="M5" s="21">
+      <c r="M5" s="16">
         <f t="shared" si="1"/>
         <v>0.9767824074074074</v>
       </c>
@@ -1767,41 +1766,41 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>44873</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>-3</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>2</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>206</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>7.8</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>85518</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>86132</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6" s="16">
         <f t="shared" si="0"/>
         <v>0.98979166666666663</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6" s="16">
         <f t="shared" si="1"/>
         <v>0.99689814814814814</v>
       </c>
@@ -1810,53 +1809,53 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="9"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="8"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="11">
-        <v>1</v>
-      </c>
-      <c r="B8" s="16">
+      <c r="A8" s="10">
+        <v>1</v>
+      </c>
+      <c r="B8" s="15">
         <v>44875</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>922</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <v>275</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <v>346</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="14">
         <v>3.1</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>65156</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="10">
         <v>66488</v>
       </c>
-      <c r="J8" s="9"/>
-      <c r="L8" s="21">
+      <c r="J8" s="8"/>
+      <c r="L8" s="16">
         <f t="shared" si="0"/>
         <v>0.75412037037037039</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M8" s="16">
         <f t="shared" si="1"/>
         <v>0.76953703703703702</v>
       </c>
@@ -1865,39 +1864,39 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>2</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="15">
         <v>44875</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>156</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <v>60</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <v>336</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>3</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>67594</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>69277</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="L9" s="21">
+      <c r="J9" s="8"/>
+      <c r="L9" s="16">
         <f t="shared" si="0"/>
         <v>0.78233796296296299</v>
       </c>
-      <c r="M9" s="21">
+      <c r="M9" s="16">
         <f t="shared" si="1"/>
         <v>0.80181712962962959</v>
       </c>
@@ -1906,39 +1905,39 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>3</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="15">
         <v>44875</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <v>276</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <v>71</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <v>328</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="14">
         <v>3.5</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <v>69964</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="10">
         <v>71461</v>
       </c>
-      <c r="J10" s="9"/>
-      <c r="L10" s="21">
+      <c r="J10" s="8"/>
+      <c r="L10" s="16">
         <f t="shared" si="0"/>
         <v>0.8097685185185185</v>
       </c>
-      <c r="M10" s="21">
+      <c r="M10" s="16">
         <f t="shared" si="1"/>
         <v>0.82709490740740743</v>
       </c>
@@ -1947,39 +1946,39 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <v>4</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="15">
         <v>44875</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>3</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>3</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <v>325</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="14">
         <v>3.9</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="10">
         <v>72299</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <v>73443</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="L11" s="21">
+      <c r="J11" s="8"/>
+      <c r="L11" s="16">
         <f t="shared" si="0"/>
         <v>0.83679398148148143</v>
       </c>
-      <c r="M11" s="21">
+      <c r="M11" s="16">
         <f t="shared" si="1"/>
         <v>0.85003472222222221</v>
       </c>
@@ -1988,39 +1987,39 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>5</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="15">
         <v>44875</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <v>31</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <v>22</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <v>329</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="14">
         <v>3.7</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="10">
         <v>74858</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="10">
         <v>76377</v>
       </c>
-      <c r="J12" s="9"/>
-      <c r="L12" s="21">
+      <c r="J12" s="8"/>
+      <c r="L12" s="16">
         <f t="shared" si="0"/>
         <v>0.86641203703703706</v>
       </c>
-      <c r="M12" s="21">
+      <c r="M12" s="16">
         <f t="shared" si="1"/>
         <v>0.88399305555555552</v>
       </c>
@@ -2029,39 +2028,39 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="11">
+      <c r="A13" s="10">
         <v>6</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="15">
         <v>44875</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <v>70</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="13">
         <v>26</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="10">
         <v>318</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="14">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="10">
         <v>77150</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="10">
         <v>78637</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="L13" s="21">
+      <c r="J13" s="8"/>
+      <c r="L13" s="16">
         <f t="shared" si="0"/>
         <v>0.89293981481481477</v>
       </c>
-      <c r="M13" s="21">
+      <c r="M13" s="16">
         <f t="shared" si="1"/>
         <v>0.91015046296296298</v>
       </c>
@@ -2070,41 +2069,41 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>7</v>
       </c>
       <c r="B14" s="3">
         <v>44875</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>7</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>10</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>318</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>4</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <v>78906</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="5">
         <v>79282</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="L14" s="21">
+      <c r="L14" s="16">
         <f t="shared" si="0"/>
         <v>0.91326388888888888</v>
       </c>
-      <c r="M14" s="21">
+      <c r="M14" s="16">
         <f t="shared" si="1"/>
         <v>0.9176157407407407</v>
       </c>
@@ -2113,53 +2112,53 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="9"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="8"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="11">
-        <v>1</v>
-      </c>
-      <c r="B16" s="16">
+      <c r="A16" s="10">
+        <v>1</v>
+      </c>
+      <c r="B16" s="15">
         <v>44876</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="11">
         <v>92</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <v>30</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="10">
         <v>25</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="14">
         <v>4.4000000000000004</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="10">
         <v>69276</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="10">
         <v>70064</v>
       </c>
-      <c r="J16" s="9"/>
-      <c r="L16" s="21">
+      <c r="J16" s="8"/>
+      <c r="L16" s="16">
         <f t="shared" si="0"/>
         <v>0.80180555555555555</v>
       </c>
-      <c r="M16" s="21">
+      <c r="M16" s="16">
         <f t="shared" si="1"/>
         <v>0.81092592592592594</v>
       </c>
@@ -2168,39 +2167,39 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="11">
+      <c r="A17" s="10">
         <v>2</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="15">
         <v>44876</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <v>3</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="13">
         <v>3</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="10">
         <v>29</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="14">
         <v>4.2</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="10">
         <v>71370</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="10">
         <v>72350</v>
       </c>
-      <c r="J17" s="9"/>
-      <c r="L17" s="21">
+      <c r="J17" s="8"/>
+      <c r="L17" s="16">
         <f t="shared" si="0"/>
         <v>0.82604166666666667</v>
       </c>
-      <c r="M17" s="21">
+      <c r="M17" s="16">
         <f t="shared" si="1"/>
         <v>0.8373842592592593</v>
       </c>
@@ -2209,41 +2208,41 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>3</v>
       </c>
       <c r="B18" s="3">
         <v>44876</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>5</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>6</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>24</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>4.4000000000000004</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <v>73526</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="5">
         <v>74522</v>
       </c>
-      <c r="J18" s="9" t="s">
+      <c r="J18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="21">
+      <c r="L18" s="16">
         <f t="shared" si="0"/>
         <v>0.85099537037037032</v>
       </c>
-      <c r="M18" s="21">
+      <c r="M18" s="16">
         <f t="shared" si="1"/>
         <v>0.86252314814814812</v>
       </c>
@@ -2252,39 +2251,39 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="11">
+      <c r="A19" s="10">
         <v>4</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="15">
         <v>44876</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <v>18</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="13">
         <v>12</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="10">
         <v>8</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="14">
         <v>3.8</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="10">
         <v>75361</v>
       </c>
-      <c r="I19" s="11">
+      <c r="I19" s="10">
         <v>76586</v>
       </c>
-      <c r="J19" s="9"/>
-      <c r="L19" s="21">
+      <c r="J19" s="8"/>
+      <c r="L19" s="16">
         <f t="shared" si="0"/>
         <v>0.87223379629629627</v>
       </c>
-      <c r="M19" s="21">
+      <c r="M19" s="16">
         <f t="shared" si="1"/>
         <v>0.88641203703703708</v>
       </c>
@@ -2293,39 +2292,39 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="11">
+      <c r="A20" s="10">
         <v>5</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="15">
         <v>44876</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="11">
         <v>0</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="13">
         <v>11</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="10">
         <v>350</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="14">
         <v>4.3</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="10">
         <v>77440</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="10">
         <v>78502</v>
       </c>
-      <c r="J20" s="9"/>
-      <c r="L20" s="21">
+      <c r="J20" s="8"/>
+      <c r="L20" s="16">
         <f t="shared" si="0"/>
         <v>0.89629629629629626</v>
       </c>
-      <c r="M20" s="21">
+      <c r="M20" s="16">
         <f t="shared" si="1"/>
         <v>0.90858796296296296</v>
       </c>
@@ -2334,39 +2333,39 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="11">
+      <c r="A21" s="10">
         <v>6</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="15">
         <v>44876</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="11">
         <v>403</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="13">
         <v>187</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="10">
         <v>351</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="14">
         <v>4.5999999999999996</v>
       </c>
-      <c r="H21" s="11">
+      <c r="H21" s="10">
         <v>81779</v>
       </c>
-      <c r="I21" s="11">
+      <c r="I21" s="10">
         <v>83042</v>
       </c>
-      <c r="J21" s="9"/>
-      <c r="L21" s="21">
+      <c r="J21" s="8"/>
+      <c r="L21" s="16">
         <f t="shared" si="0"/>
         <v>0.94651620370370371</v>
       </c>
-      <c r="M21" s="21">
+      <c r="M21" s="16">
         <f t="shared" si="1"/>
         <v>0.96113425925925922</v>
       </c>
@@ -2375,41 +2374,41 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
+      <c r="A22" s="5">
         <v>7</v>
       </c>
       <c r="B22" s="3">
         <v>44876</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>152</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>116</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <v>325</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="7">
         <v>5.3</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="5">
         <v>83871</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="5">
         <v>85173</v>
       </c>
-      <c r="J22" s="9" t="s">
+      <c r="J22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L22" s="21">
+      <c r="L22" s="16">
         <f t="shared" si="0"/>
         <v>0.97072916666666664</v>
       </c>
-      <c r="M22" s="21">
+      <c r="M22" s="16">
         <f t="shared" si="1"/>
         <v>0.98579861111111111</v>
       </c>
@@ -2419,14 +2418,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>